<commit_message>
Add other classes to sheet
</commit_message>
<xml_diff>
--- a/docs/SPFields.xlsx
+++ b/docs/SPFields.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dot Net Projects\AlAhly\dotnet-webapi-boilerplate\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DB56E8-F533-4C37-B613-F714926D016A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5CDEF5-0F44-46EE-B3B3-329F16B1EF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE581F0F-8571-454C-B86E-EACC8C1F3965}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DE581F0F-8571-454C-B86E-EACC8C1F3965}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SPFields" sheetId="1" r:id="rId1"/>
+    <sheet name="SPRelatedField" sheetId="2" r:id="rId2"/>
+    <sheet name="SPFieldTypeDefinition" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="199">
   <si>
     <t>Name</t>
   </si>
@@ -520,13 +522,195 @@
   </si>
   <si>
     <t>SPFieldLookup Members</t>
+  </si>
+  <si>
+    <t>FieldId</t>
+  </si>
+  <si>
+    <t>Gets the identifier of the lookup field in the child list.</t>
+  </si>
+  <si>
+    <t>ListId</t>
+  </si>
+  <si>
+    <t>Gets the identifier of the child list that is dependent on the parent list.</t>
+  </si>
+  <si>
+    <t>Gets the SPList object that a lookup field identifies as its target (or parent) list.</t>
+  </si>
+  <si>
+    <t>Gets the delete behavior defined by the lookup field in the child list.</t>
+  </si>
+  <si>
+    <t>WebId</t>
+  </si>
+  <si>
+    <t>Gets the identifier of the Web site where the child list is located.</t>
+  </si>
+  <si>
+    <t>AllowBaseTypeRendering</t>
+  </si>
+  <si>
+    <t>Gets a Boolean value that indicates whether a client application renders the field as its base type if the client application cannot determine how to properly render the field type.</t>
+  </si>
+  <si>
+    <t>BaseRenderingTypeName</t>
+  </si>
+  <si>
+    <t>Gets the name of the field type on which rendering of the field type definition is based.</t>
+  </si>
+  <si>
+    <t>FieldEditorUserControl</t>
+  </si>
+  <si>
+    <t>Gets the server-relative path to the control to use as a field editor control for the field type.</t>
+  </si>
+  <si>
+    <t>FieldTypeClass</t>
+  </si>
+  <si>
+    <t>Gets the full name of the class that defines the logic of the field type.</t>
+  </si>
+  <si>
+    <t>Gets a Boolean value that indicates whether the field type can be filtered.</t>
+  </si>
+  <si>
+    <t>PropertySchema</t>
+  </si>
+  <si>
+    <t>Gets the property schema that includes the set of fields that define properties that are used for the field type.</t>
+  </si>
+  <si>
+    <t>ShowOnColumnTemplateCreate</t>
+  </si>
+  <si>
+    <r>
+      <t>Gets a Boolean value that indicates whether the field type is displayed as an option on the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>New Site Column</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> page.</t>
+    </r>
+  </si>
+  <si>
+    <t>ShowOnDocumentLibraryCreate</t>
+  </si>
+  <si>
+    <r>
+      <t>Gets a Boolean value that indicates whether the field type is displayed as an option on the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Create Column</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> page for document libraries.</t>
+    </r>
+  </si>
+  <si>
+    <t>ShowOnListCreate</t>
+  </si>
+  <si>
+    <r>
+      <t>Gets a Boolean value that indicates whether the field type is displayed as an option on the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Create Column</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> page for lists.</t>
+    </r>
+  </si>
+  <si>
+    <t>ShowOnSurveyCreate</t>
+  </si>
+  <si>
+    <r>
+      <t>Gets a Boolean value that indicates whether the field type is displayed as an option on the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>New Question</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> page for surveys.</t>
+    </r>
+  </si>
+  <si>
+    <t>Gets a Boolean value that indicates whether the field type is sortable.</t>
+  </si>
+  <si>
+    <t>Gets the display name that is used to represent the field type in the user interface.</t>
+  </si>
+  <si>
+    <t>TypeName</t>
+  </si>
+  <si>
+    <t>Gets the internal name of the field type.</t>
+  </si>
+  <si>
+    <t>Gets the description of the field type.</t>
+  </si>
+  <si>
+    <t>UserCreatable</t>
+  </si>
+  <si>
+    <t>Gets a Boolean value that indicates whether users can create fields of the field type.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +726,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Segoe UI"/>
@@ -587,7 +777,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -597,13 +787,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -626,6 +816,682 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Public property">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E18430A3-B85B-1AA8-9888-8581CDB7307A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="426720"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Public property">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97EB41F9-0840-6747-7CC0-6A2FB7B96F4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="5547360"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Public property">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89E13EAF-3DE8-912C-5F23-4B9F8183CFF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="8107680"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Public property">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FE4D163-2976-A828-3D68-56C6C41CD37B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="10881360"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Public property">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B3E6F49-3ABA-9C7B-5DEA-8FC63A37B971}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="13014960"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="Public property">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0EC0551-EA9E-C2FA-C75C-6EB1A108A692}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="15148560"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="Public property">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{203E67EA-1556-01E7-EDD6-F1D87AE8597B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="18348960"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="Public property">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59E743C8-65B9-5899-F564-E2B02F5AE5CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="21762720"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="Public property">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F96E108-2ED4-5AB3-60BB-6690EC5A759B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="26029920"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="Public property">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A415CA7-A2C2-0745-0B10-E4DA0811F794}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="29657040"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="Public property">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BD10FF8-3951-0990-391C-10A51661D52D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="33284160"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -927,7 +1793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813FA763-6BB4-44D1-9C89-B5F6B3E7A287}">
   <dimension ref="A1:AA157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A124" sqref="A124:XFD124"/>
     </sheetView>
   </sheetViews>
@@ -5664,4 +6530,361 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1016"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7711F1E-C22E-400E-918D-1BA7A61388A4}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="83.44140625" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ee571148(v=office.14)" xr:uid="{A9B3EE07-7745-4790-8DE2-302AB0A131AF}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ee584778(v=office.14)" xr:uid="{E1822C30-EA8B-4DAB-AE6F-126FC37875D2}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ee542579(v=office.14)" xr:uid="{DD320A76-7D22-4BF9-ABD8-7753696B8CC2}"/>
+    <hyperlink ref="C4" r:id="rId4" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms434081(v=office.14)" xr:uid="{C9431ABA-8504-40A6-B68B-255EC6C67D68}"/>
+    <hyperlink ref="B5" r:id="rId5" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ee582649(v=office.14)" xr:uid="{C4EC48BE-C16A-4593-809B-E6AA1DAF54CC}"/>
+    <hyperlink ref="B6" r:id="rId6" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ee587116(v=office.14)" xr:uid="{26FB8D27-2777-4A02-8BDA-7F5556CCE475}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9B6860-38AE-4A8D-8AC8-2A0CF64BD403}">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="133.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2">
+        <f ca="1">D2:D10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms471876(v=office.14)" xr:uid="{41D83794-9F43-4DE9-A23C-44E3DF12B3CE}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms460375(v=office.14)" xr:uid="{A48D3B5B-D1CD-4DE3-ADDE-A4957B2A3567}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms442705(v=office.14)" xr:uid="{401CD6B9-8729-4722-BB2C-52B56B6528A4}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms452437(v=office.14)" xr:uid="{D7026CC1-9B86-4F58-AA16-E83E03DD44EB}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms461129(v=office.14)" xr:uid="{7B4C4480-D9ED-4DBD-8445-FC3B041118E2}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms469541(v=office.14)" xr:uid="{4885219D-B4DB-4C83-877C-9D1C5386106C}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms409151(v=office.14)" xr:uid="{7E160433-D854-4EB2-8381-F20D67AA6A93}"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms425589(v=office.14)" xr:uid="{FF85A517-58F8-4F36-B645-C2463F78344A}"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms436079(v=office.14)" xr:uid="{45FD45F5-62FC-4058-B5B5-91264E6A182E}"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms443997(v=office.14)" xr:uid="{B4A19E1D-A2A1-4A64-A434-F2B98B39DAD5}"/>
+    <hyperlink ref="B12" r:id="rId11" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms463730(v=office.14)" xr:uid="{5047AA2E-2D16-4C3E-B16E-F5A8A2BA6546}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms471876(v=office.14)" xr:uid="{8669E7DF-FD55-4907-A8CD-0F731F907A1E}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms460375(v=office.14)" xr:uid="{FFE9F9E5-A120-4848-A6F5-D964BCBA8A26}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms442705(v=office.14)" xr:uid="{F7825078-1ADE-4F52-9B69-2926DFE61732}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms452437(v=office.14)" xr:uid="{8F7D0460-6B1F-44A2-BCF7-671232DC470E}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms461129(v=office.14)" xr:uid="{65DA050A-CED3-447A-A27E-9D3A1ED27EEA}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms469541(v=office.14)" xr:uid="{E246636E-E3DF-437A-83EB-6FCAD71092FC}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms409151(v=office.14)" xr:uid="{FE394907-97AF-4DCF-9336-CF98A9C6701E}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms425589(v=office.14)" xr:uid="{A296E1CD-0296-49C4-A645-1332A3903CE9}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms436079(v=office.14)" xr:uid="{11B52DF4-37CA-4199-912C-ED0C5B09CBDB}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms443997(v=office.14)" xr:uid="{E4816F24-7D42-4C6E-BC92-24BE2EDFDC0C}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms463730(v=office.14)" xr:uid="{185B1B46-03F5-407B-A4ED-58E994457587}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms480835(v=office.14)" xr:uid="{B58787A2-8844-4D5B-9786-B39C701CC4FE}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms435433(v=office.14)" xr:uid="{95108F26-6B81-4CDB-B3FD-27E0BFE949B7}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms467984(v=office.14)" xr:uid="{471E52E6-CD30-4E02-80C5-C3A0E3C972B5}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://learn.microsoft.com/en-us/previous-versions/office/developer/sharepoint-2010/ms456025(v=office.14)" xr:uid="{D7DEFF07-BF00-4423-9BE2-8A4DE9470AE1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId27"/>
+</worksheet>
 </file>
</xml_diff>